<commit_message>
All capacitors selected, most other footprints assigned
</commit_message>
<xml_diff>
--- a/Powerboard/components.xlsx
+++ b/Powerboard/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2cacf5671d6b869/Desktop/PDU/Engine-Electronics/Powerboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="11_F25DC773A252ABDACC10489A811D728C5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{341FC0D0-1075-4B12-ACFF-FA5E03645D94}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="11_F25DC773A252ABDACC10489A811D728C5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE54D34E-E14C-4E32-B8FF-8CD9314FFD8E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>Price</t>
   </si>
@@ -153,7 +153,34 @@
     <t>CTTC1</t>
   </si>
   <si>
-    <t>22nf Electrolytic Cap</t>
+    <t>Min Voltage</t>
+  </si>
+  <si>
+    <t>GRM21BR61H106KE43L (at JLC)</t>
+  </si>
+  <si>
+    <t>10uF Ceramic Cap</t>
+  </si>
+  <si>
+    <t>22nf Ceramic Cap</t>
+  </si>
+  <si>
+    <t>0805(imperial)</t>
+  </si>
+  <si>
+    <t>C8,C9,C12,C13,C22,C54,C57</t>
+  </si>
+  <si>
+    <t>0603(imperial)</t>
+  </si>
+  <si>
+    <t>2.2uF Ceramic Cap</t>
+  </si>
+  <si>
+    <t>CL10B223KB8NNNC (JLC)</t>
+  </si>
+  <si>
+    <t>0805F225M500NT (JLC)</t>
   </si>
 </sst>
 </file>
@@ -539,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,6 +579,7 @@
     <col min="3" max="3" width="18.44140625" customWidth="1"/>
     <col min="4" max="4" width="133.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -571,12 +599,15 @@
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1"/>
@@ -658,7 +689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -677,7 +708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -696,7 +727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -715,7 +746,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -737,7 +768,41 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalised buck capacitors, some inital layout
</commit_message>
<xml_diff>
--- a/Powerboard/components.xlsx
+++ b/Powerboard/components.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c2cacf5671d6b869/Desktop/PDU/Engine-Electronics/Powerboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Design\ICLR Designs\PDU\Engine-Electronics\Powerboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="11_F25DC773A252ABDACC10489A811D728C5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE54D34E-E14C-4E32-B8FF-8CD9314FFD8E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Price</t>
   </si>
@@ -181,12 +180,27 @@
   </si>
   <si>
     <t>0805F225M500NT (JLC)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/Panasonic/4TPF330MFL?qs=sGAEpiMZZMsh%252B1woXyUXj9v%2FLaJorgg0K34QuPhlki8%3D</t>
+  </si>
+  <si>
+    <t>330uF Tantalum Cap</t>
+  </si>
+  <si>
+    <t>47uF Ceramic Cap</t>
+  </si>
+  <si>
+    <t>https://www.mouser.co.uk/ProductDetail/TDK/CGA9N1X7R1V476M230KC?qs=sGAEpiMZZMsh%252B1woXyUXj2GDJWaunJJjOXJcg%252BYyWqY%3D</t>
+  </si>
+  <si>
+    <t>5750(metric)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -274,7 +288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -285,6 +299,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -565,24 +582,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="133.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="133.36328125" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -615,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>18</v>
       </c>
@@ -635,7 +652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -651,7 +668,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -670,7 +687,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>25</v>
       </c>
@@ -689,7 +706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -708,7 +725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -727,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -746,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -763,7 +780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>41</v>
       </c>
@@ -777,7 +794,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>47</v>
       </c>
@@ -791,7 +808,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>40</v>
       </c>
@@ -803,19 +820,43 @@
       </c>
       <c r="E12" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="10">
+        <v>7343</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{E206F940-57B9-497B-8DDA-A1D7786D1209}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{0C3089F3-CB50-4A12-B127-132BAC414726}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{83F3225B-9B37-408C-B40E-37BBEDB609C3}"/>
-    <hyperlink ref="D5" r:id="rId4" display="https://www.mouser.co.uk/ProductDetail/Panasonic/35SVPK330M?qs=sGAEpiMZZMvwFf0viD3Y3RhiY0lA5bWmmxGvLkMUOV70WPQD0jam6A%3D%3D" xr:uid="{CCC8E311-2E89-4A81-980A-E3AC1FA738A0}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{A3F2E014-1330-4E92-ADC0-6AADFF7E1B82}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{CD35E841-5E45-4DE2-AEBC-8F82EC0E25FB}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{8F3CF623-5081-4C85-902B-0E5F18DB0884}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{172F718D-A11B-4D92-A286-C817DF1005A6}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4" display="https://www.mouser.co.uk/ProductDetail/Panasonic/35SVPK330M?qs=sGAEpiMZZMvwFf0viD3Y3RhiY0lA5bWmmxGvLkMUOV70WPQD0jam6A%3D%3D"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D7" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D13" r:id="rId9"/>
+    <hyperlink ref="D14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>